<commit_message>
update timer and schedule
</commit_message>
<xml_diff>
--- a/config/schedule.xlsx
+++ b/config/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bouki\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniwagr-my.sharepoint.com/personal/m_polychronaki_uniwa_gr/Documents/Ch_Pol Common/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43ADF0B-940A-4108-8592-7788FCD0CFB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="13_ncr:1_{F9113535-AFDD-409F-9032-89DDB0D21B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDA5557D-F2A1-47DB-BD5D-4D4D4887B304}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{5AAFB993-35D1-4E24-AA77-DA8D13F3CB42}"/>
+    <workbookView xWindow="1170" yWindow="600" windowWidth="19200" windowHeight="15600" xr2:uid="{5AAFB993-35D1-4E24-AA77-DA8D13F3CB42}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,11 +25,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
   <si>
     <t>Πρόγραμμα Διαθεσιμότητας ΖΒ109</t>
   </si>
   <si>
+    <t>Πρόγραμμα Μαθημάτων Καθηγητών</t>
+  </si>
+  <si>
     <t>ΔΕΥΤΕΡΑ</t>
   </si>
   <si>
@@ -48,295 +51,185 @@
     <t>9-10</t>
   </si>
   <si>
+    <t>Ειδικά Θέματα Δικτύων και Ασφάλεια
+ΚΟΓΙΑΣ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Θεωρία </t>
+  </si>
+  <si>
+    <t>10-11</t>
+  </si>
+  <si>
+    <t>11-12</t>
+  </si>
+  <si>
+    <t>Εργαστήριο</t>
+  </si>
+  <si>
+    <t>12-13</t>
+  </si>
+  <si>
+    <t>13-14</t>
+  </si>
+  <si>
+    <t>ΝΑΟ</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Αντικειμενοστραφής Προγραμματισμός (E)
+      <t xml:space="preserve">Ειδικά Θέματα Δικτύων και Ασφάλεια
 </t>
     </r>
     <r>
       <rPr>
         <b/>
         <sz val="10"/>
-        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Φειδάκης Μιχαήλ - 
-Λίνα Ματιάδου</t>
+      <t>Πατρικάκης Χαράλαμπος 
+ΖΒ009</t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Δίκτυα (Ε)
+      <t xml:space="preserve"> ΑΔΕ_ΕΕΕ7-2.6 
 </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="10"/>
-        <color theme="1"/>
+        <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Τσελίκης, Ουζουνίδης</t>
+      <t>Φειδάκης
+ΖΒ009</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Θεωρία </t>
-  </si>
-  <si>
-    <t>10-11</t>
-  </si>
-  <si>
-    <t>11-12</t>
+    <t>14-15</t>
+  </si>
+  <si>
+    <t>15-16</t>
+  </si>
+  <si>
+    <t>MSc AIDL</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Δίκτυα (Ε)
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve"> ΑΔΕ_ΕΕΕ7-2.6 
 </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="10"/>
-        <color theme="1"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
-      <t>Ουζουνίδης, Γαλάνη</t>
+      <t>Φειδάκης
+ΖΒ009</t>
     </r>
+  </si>
+  <si>
+    <t>16-17</t>
+  </si>
+  <si>
+    <t>17-18</t>
+  </si>
+  <si>
+    <t>Άλλο</t>
+  </si>
+  <si>
+    <t>18-19</t>
+  </si>
+  <si>
+    <t>19-20</t>
+  </si>
+  <si>
+    <t>20-21</t>
+  </si>
+  <si>
+    <t>21-22</t>
+  </si>
+  <si>
     <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Δίκτυα (Ε)
+      <t xml:space="preserve"> ΑΔΕ_ΕΕΕ7-2.6 
 </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="10"/>
-        <color theme="1"/>
+        <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Ουζουνίδης</t>
+      <t xml:space="preserve">Φειδάκης
+</t>
     </r>
   </si>
   <si>
-    <t>Εργαστήριο</t>
-  </si>
-  <si>
-    <t>12-13</t>
-  </si>
-  <si>
-    <t>13-14</t>
-  </si>
-  <si>
     <r>
-      <t xml:space="preserve">Δίκτυα (Ε)
+      <t xml:space="preserve"> ΑΔΕ_ΕΕΕ7-2.6 
 </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="10"/>
-        <color theme="1"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
-      <t>Φερλές, Ουζουνίδης</t>
+      <t xml:space="preserve">Φειδάκης
+</t>
     </r>
   </si>
   <si>
-    <t>ΝΑΟ</t>
-  </si>
-  <si>
-    <t>14-15</t>
-  </si>
-  <si>
-    <t>15-16</t>
-  </si>
-  <si>
     <r>
-      <t xml:space="preserve">Δίκτυα (Ε)
+      <t xml:space="preserve"> ΑΔΕ_ΕΕΕ7-2.6 
 </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="10"/>
-        <color theme="1"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Ουζουνίδης, Κόγιας
-</t>
+      <t>Φειδάκης-Κόγιας</t>
     </r>
   </si>
   <si>
-    <t>MSc AIDL</t>
-  </si>
-  <si>
-    <t>16-17</t>
-  </si>
-  <si>
-    <t>17-18</t>
-  </si>
-  <si>
     <r>
-      <t xml:space="preserve">AIDL_A01
- Leligou-Nikolaou
+      <t xml:space="preserve"> ΑΔΕ_ΕΕΕ7-2.6 
 </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="10"/>
-        <color theme="1"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
-      <t>ΖΒ109</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-17:00-19:15</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">AIDL_A03
-Nikolaou- Pyromalis
+      <t xml:space="preserve">Φειδάκης-Κόγιας
 </t>
     </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ΖΑ111</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-ΤΕΑΠΥ 
-Φειδακης
- </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ΖΒ208</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">AIDL_A05
-Patrikakis -invited
-&amp;
-AIDL_A06
-Patrikakis -invited
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ΖΒ109</t>
-    </r>
-  </si>
-  <si>
-    <t>Άλλο</t>
-  </si>
-  <si>
-    <t>18-19</t>
-  </si>
-  <si>
-    <t>19-20</t>
-  </si>
-  <si>
-    <t>AIDL_A02
-Κασνέσης
-19:30-22:00</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">AIDL_Α04
-Papadopoulos
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ΖΒ109</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>20-21</t>
-  </si>
-  <si>
-    <t>21-22</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,7 +261,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -376,13 +289,36 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -434,12 +370,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD5C6E4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -614,7 +544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -661,13 +591,34 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -679,28 +630,19 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1023,10 +965,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFFFC06E-2A81-4CCF-BFA3-FD697D16D73B}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,217 +977,333 @@
     <col min="2" max="6" width="23.42578125" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="15" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:15" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="21"/>
-    </row>
-    <row r="2" spans="1:8" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="28"/>
+      <c r="J1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="28"/>
+    </row>
+    <row r="2" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
       <c r="B2" s="14" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="L2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="M2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="N2" s="14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O2" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="22" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="21" t="s">
         <v>8</v>
       </c>
+      <c r="F3" s="1"/>
       <c r="H3" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="23"/>
-    </row>
-    <row r="5" spans="1:8" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="J4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="H5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="22" t="s">
+      <c r="J5" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="19"/>
+      <c r="J6" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="H7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="23"/>
-    </row>
-    <row r="7" spans="1:8" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+      <c r="J7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="M7" s="18"/>
+      <c r="N7" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="16"/>
-      <c r="H7" s="12" t="s">
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="1"/>
+      <c r="J8" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="30"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="16"/>
-    </row>
-    <row r="9" spans="1:8" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="15" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="H9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="J9" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="16"/>
-      <c r="H9" s="11" t="s">
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="19"/>
+      <c r="E10" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="J10" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="16"/>
-    </row>
-    <row r="11" spans="1:8" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="H11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="J11" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+    </row>
+    <row r="12" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="18" t="s">
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="J12" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="16"/>
+      <c r="O12" s="16"/>
+    </row>
+    <row r="13" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="27" t="s">
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="J13" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+      <c r="O13" s="16"/>
+    </row>
+    <row r="14" spans="1:15" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="J14" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="16"/>
+    </row>
+    <row r="15" spans="1:15" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="28"/>
-    </row>
-    <row r="13" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="28"/>
-      <c r="H13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="29"/>
-    </row>
-    <row r="15" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="J15" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1304,26 +1362,24 @@
       <c r="F23" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F5:F6"/>
+  <mergeCells count="15">
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="C11:C12"/>
     <mergeCell ref="D13:D15"/>
-    <mergeCell ref="A1:F1"/>
     <mergeCell ref="E7:E8"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F14"/>
   </mergeCells>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>